<commit_message>
elimnar archivo de prueba
</commit_message>
<xml_diff>
--- a/coeficientes.xlsx
+++ b/coeficientes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,7 +445,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>47.94392840425779</v>
+        <v>47.93981441118185</v>
       </c>
     </row>
     <row r="3">
@@ -453,7 +453,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>14629096554940.34</v>
+        <v>0.2707226458805622</v>
       </c>
     </row>
     <row r="4">
@@ -461,7 +461,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>9369977142826.219</v>
+        <v>-0.06386218596864779</v>
       </c>
     </row>
     <row r="5">
@@ -469,7 +469,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>17232936614768.05</v>
+        <v>0.2213498106413643</v>
       </c>
     </row>
     <row r="6">
@@ -477,7 +477,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.3156685430625201</v>
+        <v>0.3738469168289906</v>
       </c>
     </row>
     <row r="7">
@@ -485,7 +485,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.09192749696093733</v>
+        <v>0.3632458766623982</v>
       </c>
     </row>
     <row r="8">
@@ -493,7 +493,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.5792684047499642</v>
+        <v>-0.2032666004689614</v>
       </c>
     </row>
     <row r="9">
@@ -501,7 +501,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.09787550968695363</v>
+        <v>0.2027482470925074</v>
       </c>
     </row>
     <row r="10">
@@ -509,7 +509,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.09819861968648717</v>
+        <v>-0.07352680939214168</v>
       </c>
     </row>
     <row r="11">
@@ -517,7 +517,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.5487258199867339</v>
+        <v>0.1446805381226363</v>
       </c>
     </row>
     <row r="12">
@@ -525,7 +525,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.2346165273534381</v>
+        <v>0.08546923656109882</v>
       </c>
     </row>
     <row r="13">
@@ -533,7 +533,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>0.2369936461745275</v>
+        <v>0.2212358988818773</v>
       </c>
     </row>
     <row r="14">
@@ -541,7 +541,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.5415236490595625</v>
+        <v>0.05545545341961042</v>
       </c>
     </row>
     <row r="15">
@@ -549,7 +549,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.01337406648466304</v>
+        <v>-0.1106656443753674</v>
       </c>
     </row>
     <row r="16">
@@ -557,7 +557,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.2148652442933058</v>
+        <v>-0.05476329283728745</v>
       </c>
     </row>
     <row r="17">
@@ -565,7 +565,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.1419757904173976</v>
+        <v>0.6196579270378004</v>
       </c>
     </row>
     <row r="18">
@@ -573,7 +573,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.1932510218221399</v>
+        <v>0.1713491161932482</v>
       </c>
     </row>
     <row r="19">
@@ -581,7 +581,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>0.09392555329975141</v>
+        <v>0.0635071712792292</v>
       </c>
     </row>
     <row r="20">
@@ -589,7 +589,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.118988037109375</v>
+        <v>-0.1018295869040546</v>
       </c>
     </row>
     <row r="21">
@@ -597,7 +597,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.09832763671875</v>
+        <v>-0.3142911166931832</v>
       </c>
     </row>
     <row r="22">
@@ -605,15 +605,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>0.593994140625</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="n">
-        <v>0.177734375</v>
+        <v>-0.2207810511162162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>